<commit_message>
JSON Parser code 23 Mar
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="5">
   <si>
     <t>Col1</t>
   </si>
@@ -54,7 +54,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="34">
+  <fonts count="35">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -260,13 +260,29 @@
       <u val="single"/>
       <color indexed="12"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
   </fonts>
-  <fills count="64">
+  <fills count="66">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill>
@@ -591,7 +607,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
@@ -657,6 +673,8 @@
     <xf numFmtId="0" fontId="0" fillId="61" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="65" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -991,8 +1009,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.5" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.73828125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.27734375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.40625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -1095,12 +1113,15 @@
       <c r="AG1" t="s" s="64">
         <v>4</v>
       </c>
+      <c r="AH1" t="s" s="66">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="63">
+      <c r="B2" t="s" s="65">
         <v>3</v>
       </c>
     </row>
@@ -1139,6 +1160,7 @@
     <hyperlink ref="B2" r:id="rId31"/>
     <hyperlink ref="B2" r:id="rId32"/>
     <hyperlink ref="B2" r:id="rId33"/>
+    <hyperlink ref="B2" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>